<commit_message>
feat(image_handler): implement append write functionality for image-to-Excel
- Add support for appending detected tables to an existing Excel file
- Update function description to reflect new append functionality
- Improve table extraction and Excel writing process
- Maintain backward compatibility for non-append writes
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_img_input.xlsx
+++ b/src/data/input/manual/temp_img_input.xlsx
@@ -16,10 +16,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -33,7 +41,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -41,12 +49,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
feat(core): add post-processing for image to Excel conversion
- Add img_excel_after_process function in excel_handler.py
- Update main_winodw_test.py to use new post-processing function
- Modify image_to_excel process to run in
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_img_input.xlsx
+++ b/src/data/input/manual/temp_img_input.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,18 +17,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -41,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -49,33 +42,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -440,12 +415,12 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test: adjust button positions in main window layout
- Update QRect geometry values for pushButton_6, pushButton_7, pushButton_5, pushButton, and pushButton_2
- Modify vertical positions to create a more compact and organized layout
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_img_input.xlsx
+++ b/src/data/input/manual/temp_img_input.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -18,17 +18,18 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -40,12 +41,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -54,10 +70,12 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -423,20 +441,11 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
-  <cols>
-    <col width="11.625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="20.5" customWidth="1" min="2" max="2"/>
-    <col width="27.125" customWidth="1" min="3" max="3"/>
-    <col width="12.5" customWidth="1" min="4" max="4"/>
-    <col width="10.875" customWidth="1" min="5" max="5"/>
-    <col width="17.875" customWidth="1" min="6" max="6"/>
-    <col width="10.875" customWidth="1" min="8" max="8"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(excel_handler): add photo mode data commit functionality
- Extend commit_data_to_storage_excel function to support both manual and photo input modes
- Add logic to handle photo mode data by converting xlsx to xls format using xlwings library
- Update function parameters to include modle argument for identifying input mode
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_img_input.xlsx
+++ b/src/data/input/manual/temp_img_input.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -18,18 +18,17 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -41,27 +40,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -70,12 +54,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -441,11 +423,20 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
+  <cols>
+    <col width="11.625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="20.5" customWidth="1" min="2" max="2"/>
+    <col width="27.125" customWidth="1" min="3" max="3"/>
+    <col width="12.5" customWidth="1" min="4" max="4"/>
+    <col width="10.875" customWidth="1" min="5" max="5"/>
+    <col width="17.875" customWidth="1" min="6" max="6"/>
+    <col width="10.875" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(excel_handler): improve error handling and logging
- Add more specific error messages for better debugging
- Implement try-except blocks to catch and handle exceptions
- Replace hardcoded file paths with variables for better maintainability
- Add warnings for missing sheets or data instead of printing errors
- Improve logging by categorizing messages as Notice, Warning, or Error
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_img_input.xlsx
+++ b/src/data/input/manual/temp_img_input.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -18,18 +19,14 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,16 +45,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -422,20 +427,11 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
-  <cols>
-    <col width="11.625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="20.5" customWidth="1" min="2" max="2"/>
-    <col width="27.125" customWidth="1" min="3" max="3"/>
-    <col width="12.5" customWidth="1" min="4" max="4"/>
-    <col width="10.875" customWidth="1" min="5" max="5"/>
-    <col width="17.875" customWidth="1" min="6" max="6"/>
-    <col width="10.875" customWidth="1" min="8" max="8"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>